<commit_message>
Cleaning and Field 18 repeatability
Cleaned some files, finalized Field 18 repeatability and files for CS calculations
</commit_message>
<xml_diff>
--- a/Repeat score testing/2017_08_11Repeat scores from CLIC 13 18.xlsx
+++ b/Repeat score testing/2017_08_11Repeat scores from CLIC 13 18.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Dropbox\Wing project\Repeat score testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\Repeat score testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1st attempt" sheetId="1" r:id="rId1"/>
     <sheet name="2nd attempt" sheetId="2" r:id="rId2"/>
+    <sheet name="3rd attempt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="25">
   <si>
     <t>CLIC repeatability</t>
   </si>
@@ -91,6 +92,15 @@
   </si>
   <si>
     <t>Repeatability</t>
+  </si>
+  <si>
+    <t>|         SS |     70.883186 |      0.242743 |</t>
+  </si>
+  <si>
+    <t>|       * df |      1.058824 |      0.521739 |</t>
+  </si>
+  <si>
+    <t>|         MS |     75.052785 |      0.126648 |</t>
   </si>
 </sst>
 </file>
@@ -697,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:E29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,4 +968,266 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0.96542353137105996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.99831538485599502</v>
+      </c>
+      <c r="J14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.97275094820249597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>13</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="D28" s="4">
+        <v>13</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.96542353137105996</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>18</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.99831499999999995</v>
+      </c>
+      <c r="D29" s="4">
+        <v>18</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.97275094820249597</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wing check on things to make fsp presentations
Weirdness with onedrive, look into it?
Don't think many of these files were modified strongly?
</commit_message>
<xml_diff>
--- a/Repeat score testing/2017_08_11Repeat scores from CLIC 13 18.xlsx
+++ b/Repeat score testing/2017_08_11Repeat scores from CLIC 13 18.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\Repeat score testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Dropbox\Wing project\Repeat score testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1st attempt" sheetId="1" r:id="rId1"/>
     <sheet name="2nd attempt" sheetId="2" r:id="rId2"/>
-    <sheet name="3rd attempt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="22">
   <si>
     <t>CLIC repeatability</t>
   </si>
@@ -92,15 +91,6 @@
   </si>
   <si>
     <t>Repeatability</t>
-  </si>
-  <si>
-    <t>|         SS |     70.883186 |      0.242743 |</t>
-  </si>
-  <si>
-    <t>|       * df |      1.058824 |      0.521739 |</t>
-  </si>
-  <si>
-    <t>|         MS |     75.052785 |      0.126648 |</t>
   </si>
 </sst>
 </file>
@@ -707,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,266 +958,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.99970000000000003</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.96542353137105996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.99831538485599502</v>
-      </c>
-      <c r="J14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14">
-        <v>18</v>
-      </c>
-      <c r="L14" t="s">
-        <v>4</v>
-      </c>
-      <c r="O14" t="s">
-        <v>2</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0.97275094820249597</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="L15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="L18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="L20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>13</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.99970000000000003</v>
-      </c>
-      <c r="D28" s="4">
-        <v>13</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0.96542353137105996</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>18</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0.99831499999999995</v>
-      </c>
-      <c r="D29" s="4">
-        <v>18</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0.97275094820249597</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>